<commit_message>
Changed NFET, added inductors and fuses
</commit_message>
<xml_diff>
--- a/FlightBoardBOM.xlsx
+++ b/FlightBoardBOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\MatthewPoole\Documents\Post-Grad\Stanford\MS Aero-Astro\AA236B\PandaSat\electrical-documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{552CDB7F-780B-4A4A-8315-7CE7B723C4C6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61468EAD-8C46-4CAB-BC63-BCA5E3AD3AAC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="3735" windowWidth="21600" windowHeight="11385" xr2:uid="{7969AC2C-1119-489B-B180-70BBFC48BFE9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7969AC2C-1119-489B-B180-70BBFC48BFE9}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-S6C" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="328">
   <si>
     <t>Description</t>
   </si>
@@ -269,15 +269,6 @@
     <t>SOT-23</t>
   </si>
   <si>
-    <t>IRLML2803CT-ND</t>
-  </si>
-  <si>
-    <t>IRLML2803TR</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/infineon-technologies/IRLML2803TR/IRLML2803CT-ND/354727?utm_adgroup=Semiconductor%20Modules&amp;slid=&amp;gclid=CjwKCAiAv9riBRANEiwA9Dqv1dEeynYGSZ1Z-8vVvoxYSLaO6JjboIfXfgzu60ACLyAF1VSy52zfGxoCpNQQAvD_BwE</t>
-  </si>
-  <si>
     <t>P-Channel MOSFET</t>
   </si>
   <si>
@@ -473,21 +464,12 @@
     <t>Inductors</t>
   </si>
   <si>
-    <t>L1,L2,L3</t>
-  </si>
-  <si>
     <t>Fuses</t>
   </si>
   <si>
-    <t>F1,F2</t>
-  </si>
-  <si>
     <t>Jumper</t>
   </si>
   <si>
-    <t>JP1,JP2,JP3,JP4,JP5,JP6</t>
-  </si>
-  <si>
     <t>https://www.mouser.com/ProductDetail/Molex/22-28-4027?qs=sGAEpiMZZMs%252bGHln7q6pm%252bS0pk2Wo0XxNI9H%252bWJw8G8%3d</t>
   </si>
   <si>
@@ -500,21 +482,6 @@
     <t>2 Position Male Jumper</t>
   </si>
   <si>
-    <t>3 Position Male Jumper</t>
-  </si>
-  <si>
-    <t>JP7,JP8,JP9</t>
-  </si>
-  <si>
-    <t>649-68004-103HLF</t>
-  </si>
-  <si>
-    <t>68004-103HLF</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/Amphenol-FCI/68004-103HLF?qs=sGAEpiMZZMs%252bGHln7q6pm2nKUjHUi6l6jmnOf127njY%3d</t>
-  </si>
-  <si>
     <t>Resistors</t>
   </si>
   <si>
@@ -957,6 +924,96 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/infineon-technologies/IRLML2803TRPBF/IRLML2803PBFCT-ND/812498</t>
+  </si>
+  <si>
+    <t>IRLML2803PBFCT-ND</t>
+  </si>
+  <si>
+    <t>IRLML2803TRPBF</t>
+  </si>
+  <si>
+    <t>JP6,JP7,JP8,JP9</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>2-SMD</t>
+  </si>
+  <si>
+    <t>SMD300F-2CT-ND</t>
+  </si>
+  <si>
+    <t>SMD300F-2</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/littelfuse-inc/SMD300F-2/SMD300F-2CT-ND/1045852</t>
+  </si>
+  <si>
+    <t>J14,J15,J16</t>
+  </si>
+  <si>
+    <t>2 Pin Molex Vertical 2.54mm pitch</t>
+  </si>
+  <si>
+    <t>A1921-ND</t>
+  </si>
+  <si>
+    <t>640456-2</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/640456-2/A1921-ND/109003</t>
+  </si>
+  <si>
+    <t>56uH Fixed Inductor</t>
+  </si>
+  <si>
+    <t>652-CM322522-560KL</t>
+  </si>
+  <si>
+    <t>CM322522-560KL</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Bourns/CM322522-560KL?qs=sGAEpiMZZMsg%252by3WlYCkU45muCuneYXkqlGCquKUX0k%3d</t>
+  </si>
+  <si>
+    <t>10uH Fixed Inductor</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>652-CM322522-100KL</t>
+  </si>
+  <si>
+    <t>CM322522-100KL</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Bourns/CM322522-100KL?qs=sGAEpiMZZMsg%252by3WlYCkU45muCuneYXkVwLPC%2fVldao%3d</t>
+  </si>
+  <si>
+    <t>3.3uH Fixed Inductor</t>
+  </si>
+  <si>
+    <t>L3</t>
+  </si>
+  <si>
+    <t>652-CM322522-3R3KL</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Bourns/CM453232-3R3KL?qs=sGAEpiMZZMsg%252by3WlYCkU%252b4RYdUJmhyQLuAED5QNU9M%3d</t>
+  </si>
+  <si>
+    <t>CM453232-3R3KL</t>
+  </si>
+  <si>
+    <t>6V 3A Reset Fuse</t>
   </si>
 </sst>
 </file>
@@ -1103,6 +1160,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1112,8 +1171,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1429,10 +1486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C3A4314-0F82-4785-B06F-435A11FFC277}">
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="H75" sqref="H75"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1472,16 +1529,16 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="8"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="10"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1744,16 +1801,16 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="8"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -1782,16 +1839,16 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="8"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -1807,13 +1864,13 @@
         <v>4</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>79</v>
+        <v>299</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>80</v>
+        <v>300</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>81</v>
+        <v>298</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>29</v>
@@ -1821,10 +1878,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>59</v>
@@ -1833,115 +1890,115 @@
         <v>3</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>29</v>
+        <v>297</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" s="3">
+        <v>1</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="G18" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D18" s="3">
-        <v>1</v>
-      </c>
-      <c r="E18" s="4" t="s">
+      <c r="H18" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="8"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="G20" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D20" s="3">
-        <v>1</v>
-      </c>
-      <c r="E20" s="4" t="s">
+      <c r="H20" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="8"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D22" s="3">
         <v>2</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>29</v>
@@ -1949,1085 +2006,1161 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="G23" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="D23" s="3">
-        <v>1</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="8"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D25" s="3">
         <v>1</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F25" s="2">
         <v>5031821852</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D26" s="3">
         <v>1</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D27" s="3">
         <v>1</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D28" s="3">
         <v>1</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F28" s="2">
         <v>132134</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D29" s="3">
+        <v>1</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="D29" s="3">
-        <v>1</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>140</v>
-      </c>
       <c r="F29" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D30" s="3">
         <v>8</v>
       </c>
       <c r="E30" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D31" s="3">
+        <v>3</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="10"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="C33" s="2">
+        <v>1210</v>
+      </c>
+      <c r="D33" s="3">
+        <v>1</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="C34" s="2">
+        <v>1210</v>
+      </c>
+      <c r="D34" s="3">
+        <v>1</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C35" s="2">
+        <v>1210</v>
+      </c>
+      <c r="D35" s="3">
+        <v>1</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="G30" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="8"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="8"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="8"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D36" s="3">
-        <v>6</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>308</v>
-      </c>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="10"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>155</v>
+        <v>327</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>157</v>
+        <v>302</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>137</v>
+        <v>303</v>
       </c>
       <c r="D37" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>153</v>
+        <v>304</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>154</v>
+        <v>305</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>152</v>
+        <v>306</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="8"/>
+      <c r="A38" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="10"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>179</v>
+        <v>301</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>185</v>
+        <v>134</v>
       </c>
       <c r="D39" s="3">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>204</v>
+        <v>147</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>187</v>
+        <v>148</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>203</v>
+        <v>146</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="D40" s="3">
-        <v>7</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>308</v>
-      </c>
+      <c r="A40" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="10"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="D41" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="G41" s="9" t="s">
-        <v>200</v>
+        <v>176</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>192</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>185</v>
-      </c>
       <c r="D42" s="3">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="D43" s="3">
         <v>1</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>192</v>
+        <v>178</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>189</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="D44" s="3">
         <v>4</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="C45" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D45" s="3">
+        <v>1</v>
+      </c>
+      <c r="E45" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="D45" s="3">
-        <v>1</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>205</v>
-      </c>
       <c r="F45" s="2" t="s">
-        <v>206</v>
+        <v>180</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>207</v>
+        <v>181</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="D46" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>208</v>
+        <v>182</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>209</v>
+        <v>183</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>210</v>
+        <v>184</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="D47" s="3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="D48" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="D49" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>219</v>
+        <v>202</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
-      <c r="G50" s="7"/>
-      <c r="H50" s="8"/>
+      <c r="A50" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D50" s="3">
+        <v>2</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>220</v>
+        <v>172</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>221</v>
+        <v>173</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="D51" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>254</v>
+        <v>206</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>255</v>
+        <v>207</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>256</v>
+        <v>208</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="D52" s="3">
-        <v>1</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="G52" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>308</v>
-      </c>
+      <c r="A52" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B52" s="9"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="9"/>
+      <c r="H52" s="10"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>239</v>
+        <v>210</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="D53" s="3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>260</v>
+        <v>243</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="G53" s="9" t="s">
-        <v>262</v>
+        <v>244</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>245</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="D54" s="3">
         <v>1</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>264</v>
+        <v>246</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>265</v>
+        <v>247</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>266</v>
+        <v>248</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="I54" s="10" t="s">
-        <v>263</v>
+        <v>297</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>228</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="D55" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>269</v>
+        <v>250</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>251</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>242</v>
+        <v>215</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="D56" s="3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>270</v>
+        <v>253</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
+      </c>
+      <c r="I56" s="7" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="D57" s="3">
         <v>1</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>274</v>
+        <v>257</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>275</v>
+        <v>258</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>307</v>
+        <v>231</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="D58" s="3">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="D59" s="3">
         <v>1</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>236</v>
+        <v>296</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="D60" s="3">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>282</v>
+        <v>265</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>284</v>
+        <v>267</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="D61" s="3">
         <v>1</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>285</v>
+        <v>268</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>286</v>
+        <v>269</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>287</v>
+        <v>270</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>240</v>
+        <v>224</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="D62" s="3">
         <v>1</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>289</v>
+        <v>271</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>290</v>
+        <v>272</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>291</v>
+        <v>273</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="I62" s="10" t="s">
-        <v>288</v>
+        <v>297</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>248</v>
+        <v>226</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="D63" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>292</v>
+        <v>274</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>293</v>
+        <v>275</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>249</v>
+        <v>229</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="D64" s="3">
         <v>1</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>295</v>
+        <v>278</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>296</v>
+        <v>279</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>297</v>
+        <v>280</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
+      </c>
+      <c r="I64" s="7" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>246</v>
+        <v>174</v>
       </c>
       <c r="D65" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>304</v>
+        <v>281</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>305</v>
+        <v>282</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>306</v>
+        <v>283</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="D66" s="3">
         <v>1</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>253</v>
+        <v>234</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>185</v>
+        <v>235</v>
       </c>
       <c r="D67" s="3">
         <v>1</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D68" s="3">
+        <v>1</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D69" s="3">
+        <v>1</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>297</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A50:H50"/>
-    <mergeCell ref="A24:H24"/>
-    <mergeCell ref="A31:H31"/>
-    <mergeCell ref="A33:H33"/>
-    <mergeCell ref="A35:H35"/>
-    <mergeCell ref="A38:H38"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A13:H13"/>
     <mergeCell ref="A15:H15"/>
     <mergeCell ref="A19:H19"/>
     <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A52:H52"/>
+    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="A32:H32"/>
+    <mergeCell ref="A36:H36"/>
+    <mergeCell ref="A38:H38"/>
+    <mergeCell ref="A40:H40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Corrected foot/rail switch parts
</commit_message>
<xml_diff>
--- a/FlightBoardBOM.xlsx
+++ b/FlightBoardBOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\MatthewPoole\Documents\Post-Grad\Stanford\MS Aero-Astro\AA236B\PandaSat\electrical-documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F2A88A-164E-41AD-8F06-42F2E0B4375B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DFA11B7-E947-4327-AE4C-CA41CEB231FC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4785" yWindow="4080" windowWidth="21600" windowHeight="11385" xr2:uid="{7969AC2C-1119-489B-B180-70BBFC48BFE9}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{7969AC2C-1119-489B-B180-70BBFC48BFE9}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-S6C" sheetId="1" r:id="rId1"/>
@@ -878,15 +878,6 @@
     <t>J14,J15,J16</t>
   </si>
   <si>
-    <t>2 Pin Molex Vertical 2.54mm pitch</t>
-  </si>
-  <si>
-    <t>A1921-ND</t>
-  </si>
-  <si>
-    <t>640456-2</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/640456-2/A1921-ND/109003</t>
   </si>
   <si>
@@ -1014,6 +1005,15 @@
   </si>
   <si>
     <t>https://www.mouser.com/ProductDetail/ON-Semiconductor/BC846BLT1G?qs=sGAEpiMZZMtqO%252bWUGLBzePo0Ry%252bsrgua</t>
+  </si>
+  <si>
+    <t>2 Pin Screw Terminals 3.5mm Pitch</t>
+  </si>
+  <si>
+    <t>474-PRT-08084</t>
+  </si>
+  <si>
+    <t>PRT-08084</t>
   </si>
 </sst>
 </file>
@@ -1488,8 +1488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C3A4314-0F82-4785-B06F-435A11FFC277}">
   <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:H18"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1606,13 +1606,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>38</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>29</v>
@@ -1632,13 +1632,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>29</v>
@@ -1762,13 +1762,13 @@
         <v>1</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>29</v>
@@ -1916,13 +1916,13 @@
         <v>1</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>271</v>
@@ -2073,7 +2073,7 @@
         <v>102</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>117</v>
@@ -2102,19 +2102,19 @@
         <v>108</v>
       </c>
       <c r="C27" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="D27" s="3">
+        <v>1</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="G27" s="2" t="s">
         <v>318</v>
-      </c>
-      <c r="D27" s="3">
-        <v>1</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>319</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>321</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>271</v>
@@ -2177,7 +2177,7 @@
         <v>106</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>118</v>
@@ -2200,7 +2200,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>282</v>
+        <v>325</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>281</v>
@@ -2212,13 +2212,13 @@
         <v>3</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>283</v>
+        <v>326</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>284</v>
+        <v>327</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>271</v>
@@ -2238,10 +2238,10 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C33" s="2">
         <v>1210</v>
@@ -2250,13 +2250,13 @@
         <v>1</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>271</v>
@@ -2264,10 +2264,10 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C34" s="2">
         <v>1210</v>
@@ -2276,13 +2276,13 @@
         <v>1</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>271</v>
@@ -2290,10 +2290,10 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C35" s="2">
         <v>1210</v>
@@ -2302,13 +2302,13 @@
         <v>1</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>271</v>
@@ -2328,7 +2328,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>276</v>
@@ -2676,13 +2676,13 @@
         <v>5</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="H51" s="2" t="s">
         <v>271</v>
@@ -2792,19 +2792,19 @@
         <v>1</v>
       </c>
       <c r="E56" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="I56" s="7" t="s">
         <v>309</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="I56" s="7" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -3003,13 +3003,13 @@
         <v>1</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="H64" s="2" t="s">
         <v>271</v>
@@ -3150,17 +3150,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="A21:H21"/>
     <mergeCell ref="A52:H52"/>
     <mergeCell ref="A24:H24"/>
     <mergeCell ref="A32:H32"/>
     <mergeCell ref="A36:H36"/>
     <mergeCell ref="A38:H38"/>
     <mergeCell ref="A40:H40"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A13:H13"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A21:H21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>